<commit_message>
AT: minor script revisions during data exploration, nothing substantial
</commit_message>
<xml_diff>
--- a/results/initial_descriptives/NRI/pcnt_landu_by_lcc.xlsx
+++ b/results/initial_descriptives/NRI/pcnt_landu_by_lcc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\GitRepos\land-use\results\initial_descriptives\NRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3EB4D1-5C5C-45AE-A858-9463533B3B69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5DF39F-E6C8-4E51-8AE2-3D430E9FB031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1982" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="2007" sheetId="6" r:id="rId6"/>
     <sheet name="2012" sheetId="7" r:id="rId7"/>
     <sheet name="mean" sheetId="8" r:id="rId8"/>
+    <sheet name="readme" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="22">
   <si>
     <t>year</t>
   </si>
@@ -87,6 +88,12 @@
   </si>
   <si>
     <t>Waterland</t>
+  </si>
+  <si>
+    <t>Tables add up to 100%</t>
+  </si>
+  <si>
+    <t>Interpretation: X% of ALL LAND is in land use A AND in LCC B</t>
   </si>
 </sst>
 </file>
@@ -3001,8 +3008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3330,4 +3337,29 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7CA3B3-BA7E-4B9C-89C6-F8C2A8EE4855}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>